<commit_message>
Added some test cases related to travellers
</commit_message>
<xml_diff>
--- a/DataSheets/Data_sheets_expedia.xlsx
+++ b/DataSheets/Data_sheets_expedia.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Selenium\Selenium projects\Expedia_automation\Data_sheets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Selenium\Selenium projects second\ExpediaMavenFramework\DataSheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3717636C-F4D1-45F1-98E5-F104C259E923}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73AADF02-81B2-4F06-B1B5-7821E74DAF9E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Important Information" sheetId="6" r:id="rId1"/>
-    <sheet name="OneWayFlightsPosTravellers" sheetId="3" r:id="rId2"/>
+    <sheet name="OneWayFlightsPosTrvDate" sheetId="3" r:id="rId2"/>
     <sheet name="OneWayFlightsPosDefaultDate" sheetId="4" r:id="rId3"/>
     <sheet name="OneWayFlightsPosDate" sheetId="5" r:id="rId4"/>
-    <sheet name="FlightsOnlyPosWAge" sheetId="1" r:id="rId5"/>
+    <sheet name="OneWayFlightsWithTravellers" sheetId="1" r:id="rId5"/>
     <sheet name="FlightsWithHotelsPositive" sheetId="2" r:id="rId6"/>
   </sheets>
   <calcPr calcId="0"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="57">
   <si>
     <t>OneWayHotels</t>
   </si>
@@ -87,10 +87,6 @@
     <t>Delhi</t>
   </si>
   <si>
-    <t>Instruction - Put the start tag (One-way) before the first column and the first row to be used and the end tag (One-way) after the last column and last row to be used.
-Only use future dates here.</t>
-  </si>
-  <si>
     <t>AdultNos</t>
   </si>
   <si>
@@ -98,18 +94,6 @@
   </si>
   <si>
     <t>InfantNos</t>
-  </si>
-  <si>
-    <t>ChildrenAges</t>
-  </si>
-  <si>
-    <t>InfantAges</t>
-  </si>
-  <si>
-    <t>Under1,1</t>
-  </si>
-  <si>
-    <t>2,4,8</t>
   </si>
   <si>
     <r>
@@ -140,33 +124,12 @@
     <t>06/09/2020</t>
   </si>
   <si>
-    <t>20 Sep 2020</t>
-  </si>
-  <si>
-    <t>OneWayAge</t>
-  </si>
-  <si>
-    <t>25 Sep 2020</t>
-  </si>
-  <si>
-    <t>01 Jan 2021</t>
-  </si>
-  <si>
-    <t>27 Dec 2020</t>
-  </si>
-  <si>
     <t>19 Nov 2020</t>
   </si>
   <si>
     <t>7 Jan 2021</t>
   </si>
   <si>
-    <t>12 Jan 2021</t>
-  </si>
-  <si>
-    <t>OneWayFlightsTravellers</t>
-  </si>
-  <si>
     <t>Kozhikode</t>
   </si>
   <si>
@@ -180,6 +143,63 @@
   </si>
   <si>
     <t>Date</t>
+  </si>
+  <si>
+    <t>Hyderabad</t>
+  </si>
+  <si>
+    <t>New Delhi</t>
+  </si>
+  <si>
+    <t>Bangkok</t>
+  </si>
+  <si>
+    <t>Kolkata</t>
+  </si>
+  <si>
+    <t>Tokyo</t>
+  </si>
+  <si>
+    <t>Chicago</t>
+  </si>
+  <si>
+    <t>Bangalore</t>
+  </si>
+  <si>
+    <t>Bombay</t>
+  </si>
+  <si>
+    <t>Bhubaneswar</t>
+  </si>
+  <si>
+    <t>6 Jun 2021</t>
+  </si>
+  <si>
+    <t>3 May 2021</t>
+  </si>
+  <si>
+    <t>25 Apr 2021</t>
+  </si>
+  <si>
+    <t>18 Aug 2021</t>
+  </si>
+  <si>
+    <t>28 Mar 2021</t>
+  </si>
+  <si>
+    <t>OneWayTravellers</t>
+  </si>
+  <si>
+    <t>Instruction - Put the start tag (OneWayFlightsPosDate) before the first column and the first row to be used and the end tag (OneWayFlightsPosDate) after the last column and last row to be used.
+Only use positive scenarios here.</t>
+  </si>
+  <si>
+    <t>Instruction - Put the start tag (OneWayTravellers) before the first column and the first row to be used and the end tag (OneWayTravellers) after the last column and last row to be used.
+Only use positive scenarios here.</t>
+  </si>
+  <si>
+    <t>Instruction - Put the start tag (OneWayFlightsPos) before the first column and the first row to be used and the end tag (OneWayFlightsPos) after the last column and last row to be used.
+Only use positive scenarios here.</t>
   </si>
   <si>
     <r>
@@ -195,54 +215,34 @@
       </rPr>
       <t>Don't provide past dates else the test will fail.</t>
     </r>
-  </si>
-  <si>
-    <t>Hyderabad</t>
-  </si>
-  <si>
-    <t>New Delhi</t>
-  </si>
-  <si>
-    <t>Bangkok</t>
-  </si>
-  <si>
-    <t>Kolkata</t>
-  </si>
-  <si>
-    <t>Tokyo</t>
-  </si>
-  <si>
-    <t>Chicago</t>
-  </si>
-  <si>
-    <t>Bangalore</t>
-  </si>
-  <si>
-    <t>Bombay</t>
-  </si>
-  <si>
-    <t>Bhubaneswar</t>
-  </si>
-  <si>
-    <t>6 Jun 2021</t>
-  </si>
-  <si>
-    <t>3 May 2021</t>
-  </si>
-  <si>
-    <t>7 Mar 2021</t>
-  </si>
-  <si>
-    <t>28 Feb 2021</t>
-  </si>
-  <si>
-    <t>25 Apr 2021</t>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+Look out for specific instruction in each sheet.</t>
+    </r>
+  </si>
+  <si>
+    <t>12 Jun 2021</t>
+  </si>
+  <si>
+    <t>30 Mar 2021</t>
+  </si>
+  <si>
+    <t>OneWayFlightsTravellersDate</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="[$-14009]dd\ mmmm\ yyyy;@"/>
+  </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -307,7 +307,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -316,6 +316,8 @@
     <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -555,30 +557,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1" s="8" t="s">
-        <v>47</v>
+      <c r="A1" s="10" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" s="9"/>
+      <c r="A2" s="11"/>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A3" s="9"/>
+      <c r="A3" s="11"/>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A4" s="9"/>
+      <c r="A4" s="11"/>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A5" s="9"/>
+      <c r="A5" s="11"/>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A6" s="9"/>
+      <c r="A6" s="11"/>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A7" s="9"/>
+      <c r="A7" s="11"/>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A8" s="9"/>
+      <c r="A8" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -591,10 +593,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD5D1D3A-5071-4574-BCCD-29CCFD49D1EA}">
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:M11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -602,11 +604,13 @@
     <col min="1" max="1" width="24.33203125" customWidth="1"/>
     <col min="2" max="7" width="13.08203125" customWidth="1"/>
     <col min="8" max="8" width="22.4140625" customWidth="1"/>
+    <col min="12" max="12" width="18" customWidth="1"/>
+    <col min="13" max="13" width="18.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
-        <v>41</v>
+    <row r="1" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A1" s="9" t="s">
+        <v>56</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -618,16 +622,16 @@
         <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="G1" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
       <c r="B2" s="1" t="s">
         <v>13</v>
       </c>
@@ -635,7 +639,7 @@
         <v>4</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>40</v>
+        <v>54</v>
       </c>
       <c r="E2">
         <v>2</v>
@@ -647,7 +651,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
       <c r="B3" s="1" t="s">
         <v>12</v>
       </c>
@@ -655,7 +659,7 @@
         <v>16</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>35</v>
+        <v>46</v>
       </c>
       <c r="E3">
         <v>4</v>
@@ -666,11 +670,8 @@
       <c r="G3">
         <v>0</v>
       </c>
-      <c r="H3" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="4" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
       <c r="B4" s="1" t="s">
         <v>18</v>
       </c>
@@ -678,7 +679,7 @@
         <v>7</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>37</v>
+        <v>55</v>
       </c>
       <c r="E4">
         <v>1</v>
@@ -690,7 +691,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
       <c r="B5" s="1" t="s">
         <v>7</v>
       </c>
@@ -698,7 +699,7 @@
         <v>14</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="E5">
         <v>1</v>
@@ -710,7 +711,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
       <c r="B6" s="1" t="s">
         <v>19</v>
       </c>
@@ -718,7 +719,7 @@
         <v>17</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="E6">
         <v>1</v>
@@ -730,17 +731,37 @@
         <v>0</v>
       </c>
     </row>
+    <row r="7" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="H7" s="9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="54" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F10" s="8"/>
+      <c r="L10" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="M10" s="12"/>
+    </row>
+    <row r="11" spans="1:13" ht="60.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="L11" s="12"/>
+      <c r="M11" s="12"/>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="L10:M11"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA583240-635E-4608-A31D-5DD5BA037B77}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:J10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I9" sqref="I9:J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -749,11 +770,13 @@
     <col min="2" max="2" width="12.08203125" customWidth="1"/>
     <col min="3" max="3" width="17.33203125" customWidth="1"/>
     <col min="4" max="4" width="16.5" customWidth="1"/>
+    <col min="9" max="9" width="21.83203125" customWidth="1"/>
+    <col min="10" max="10" width="18.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -762,52 +785,67 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="C2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B3" s="7" t="s">
-        <v>48</v>
+        <v>35</v>
       </c>
       <c r="C3" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D3" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B4" s="7" t="s">
-        <v>49</v>
+        <v>36</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B5" s="7" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="C5" s="7" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="D6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="33.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I9" s="12" t="s">
         <v>52</v>
       </c>
+      <c r="J9" s="12"/>
+    </row>
+    <row r="10" spans="1:10" ht="73" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I10" s="12"/>
+      <c r="J10" s="12"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="I9:J10"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A0505F9-B8CF-4B2F-A121-89B24FCC7D64}">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="J9" sqref="J9:K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -816,11 +854,13 @@
     <col min="2" max="2" width="12" customWidth="1"/>
     <col min="3" max="4" width="14.33203125" customWidth="1"/>
     <col min="5" max="5" width="23.5" customWidth="1"/>
+    <col min="10" max="10" width="18.4140625" customWidth="1"/>
+    <col min="11" max="11" width="13.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -829,21 +869,21 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="14.5" x14ac:dyDescent="0.35">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="14.5" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="C2" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="14.5" x14ac:dyDescent="0.35">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="14.5" x14ac:dyDescent="0.35">
       <c r="B3" s="7" t="s">
         <v>4</v>
       </c>
@@ -851,79 +891,91 @@
         <v>14</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="14.5" x14ac:dyDescent="0.35">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="14.5" x14ac:dyDescent="0.35">
       <c r="B4" s="7" t="s">
         <v>7</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="14.5" x14ac:dyDescent="0.35">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="14.5" x14ac:dyDescent="0.35">
       <c r="B5" s="7" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="14.5" x14ac:dyDescent="0.35">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="14.5" x14ac:dyDescent="0.35">
       <c r="B6" s="7" t="s">
-        <v>56</v>
+        <v>43</v>
       </c>
       <c r="C6" s="7" t="s">
         <v>19</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="E7" t="s">
-        <v>45</v>
-      </c>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="38.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J9" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="K9" s="12"/>
+    </row>
+    <row r="10" spans="1:11" ht="58.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J10" s="12"/>
+      <c r="K10" s="12"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="J9:K10"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J1000"/>
+  <dimension ref="A1:I1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="H8" sqref="H8:I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.6640625" customWidth="1"/>
+    <col min="1" max="1" width="17.25" customWidth="1"/>
     <col min="2" max="2" width="12.6640625" customWidth="1"/>
     <col min="3" max="3" width="15.6640625" customWidth="1"/>
-    <col min="4" max="4" width="24.5" customWidth="1"/>
-    <col min="5" max="5" width="14.58203125" customWidth="1"/>
-    <col min="6" max="6" width="16.25" customWidth="1"/>
-    <col min="7" max="7" width="24.4140625" customWidth="1"/>
-    <col min="8" max="8" width="26.33203125" customWidth="1"/>
-    <col min="9" max="10" width="27.25" customWidth="1"/>
-    <col min="11" max="11" width="26.4140625" customWidth="1"/>
-    <col min="12" max="12" width="26" customWidth="1"/>
-    <col min="13" max="26" width="7.6640625" customWidth="1"/>
+    <col min="4" max="4" width="14.58203125" customWidth="1"/>
+    <col min="5" max="5" width="16.25" customWidth="1"/>
+    <col min="6" max="6" width="24.4140625" customWidth="1"/>
+    <col min="7" max="7" width="26.33203125" customWidth="1"/>
+    <col min="8" max="9" width="27.25" customWidth="1"/>
+    <col min="10" max="10" width="26.4140625" customWidth="1"/>
+    <col min="11" max="11" width="26" customWidth="1"/>
+    <col min="12" max="25" width="7.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>34</v>
+        <v>49</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -931,8 +983,8 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
+      <c r="D1" s="2" t="s">
+        <v>20</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>21</v>
@@ -940,144 +992,116 @@
       <c r="F1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="G1" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+    </row>
+    <row r="2" spans="1:9" ht="17" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B2" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="6" t="s">
-        <v>33</v>
+      <c r="D2">
+        <v>2</v>
       </c>
       <c r="E2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F2">
         <v>1</v>
       </c>
-      <c r="G2">
-        <v>1</v>
-      </c>
-      <c r="H2" t="s">
-        <v>27</v>
-      </c>
-      <c r="I2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="3" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B3" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="6" t="s">
-        <v>35</v>
+      <c r="D3">
+        <v>4</v>
       </c>
       <c r="E3">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="F3">
         <v>1</v>
       </c>
-      <c r="G3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="4" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B4" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="6" t="s">
-        <v>37</v>
+      <c r="D4">
+        <v>3</v>
       </c>
       <c r="E4">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F4">
         <v>2</v>
       </c>
-      <c r="G4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="5" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B5" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="6" t="s">
-        <v>38</v>
+      <c r="D5">
+        <v>3</v>
       </c>
       <c r="E5">
+        <v>2</v>
+      </c>
+      <c r="F5">
         <v>1</v>
       </c>
-      <c r="F5">
-        <v>0</v>
-      </c>
-      <c r="G5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="6" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B6" s="1" t="s">
         <v>19</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="6" t="s">
-        <v>36</v>
+      <c r="D6">
+        <v>6</v>
       </c>
       <c r="E6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F6">
         <v>0</v>
       </c>
-      <c r="G6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="14" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="J7" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" ht="49.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="I8" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="J8" s="10"/>
-    </row>
-    <row r="9" spans="1:10" ht="27.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="I9" s="10"/>
-      <c r="J9" s="10"/>
-    </row>
-    <row r="10" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="11" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="12" spans="1:10" ht="31.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="13" spans="1:10" ht="46" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="14" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="15" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="16" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    </row>
+    <row r="7" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G7" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="49.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H8" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="I8" s="12"/>
+    </row>
+    <row r="9" spans="1:9" ht="27.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H9" s="12"/>
+      <c r="I9" s="12"/>
+    </row>
+    <row r="10" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="11" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="12" spans="1:9" ht="31.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="13" spans="1:9" ht="46" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="14" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="15" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="16" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="17" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="18" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2064,7 +2088,7 @@
     <row r="1000" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="I8:J9"/>
+    <mergeCell ref="H8:I9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="portrait"/>
@@ -2120,13 +2144,13 @@
         <v>9</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
@@ -2137,13 +2161,13 @@
         <v>10</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>0</v>
@@ -2160,22 +2184,22 @@
         <v>11</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="14" x14ac:dyDescent="0.3"/>
     <row r="11" spans="1:8" ht="49.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G11" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="H11" s="10"/>
+      <c r="G11" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="H11" s="12"/>
     </row>
     <row r="12" spans="1:8" ht="34" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G12" s="10"/>
-      <c r="H12" s="10"/>
+      <c r="G12" s="12"/>
+      <c r="H12" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
corrected a date in the data sheet.
</commit_message>
<xml_diff>
--- a/DataSheets/Data_sheets_expedia.xlsx
+++ b/DataSheets/Data_sheets_expedia.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Selenium\Selenium projects second\ExpediaMavenFramework\DataSheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73AADF02-81B2-4F06-B1B5-7821E74DAF9E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AC3BF23-2D3E-47C5-8CE2-C83E9758A650}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Important Information" sheetId="6" r:id="rId1"/>
@@ -122,9 +122,6 @@
   </si>
   <si>
     <t>06/09/2020</t>
-  </si>
-  <si>
-    <t>19 Nov 2020</t>
   </si>
   <si>
     <t>7 Jan 2021</t>
@@ -234,6 +231,9 @@
   </si>
   <si>
     <t>OneWayFlightsTravellersDate</t>
+  </si>
+  <si>
+    <t>19 Nov 2021</t>
   </si>
 </sst>
 </file>
@@ -558,7 +558,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="10" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
@@ -596,7 +596,7 @@
   <dimension ref="A1:M11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -610,7 +610,7 @@
   <sheetData>
     <row r="1" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A1" s="9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -639,7 +639,7 @@
         <v>4</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E2">
         <v>2</v>
@@ -659,7 +659,7 @@
         <v>16</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E3">
         <v>4</v>
@@ -679,7 +679,7 @@
         <v>7</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E4">
         <v>1</v>
@@ -699,7 +699,7 @@
         <v>14</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>28</v>
+        <v>56</v>
       </c>
       <c r="E5">
         <v>1</v>
@@ -719,7 +719,7 @@
         <v>17</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E6">
         <v>1</v>
@@ -733,13 +733,13 @@
     </row>
     <row r="7" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
       <c r="H7" s="9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="10" spans="1:13" ht="54" customHeight="1" x14ac:dyDescent="0.3">
       <c r="F10" s="8"/>
       <c r="L10" s="12" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="M10" s="12"/>
     </row>
@@ -776,7 +776,7 @@
   <sheetData>
     <row r="1" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -787,15 +787,15 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" t="s">
         <v>30</v>
-      </c>
-      <c r="C2" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B3" s="7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C3" s="7" t="s">
         <v>10</v>
@@ -803,28 +803,28 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B4" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C4" s="7" t="s">
         <v>36</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B5" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C5" s="7" t="s">
         <v>38</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="D6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="33.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="I9" s="12" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="J9" s="12"/>
     </row>
@@ -860,7 +860,7 @@
   <sheetData>
     <row r="1" spans="1:11" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -869,18 +869,18 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="14.5" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" t="s">
         <v>30</v>
       </c>
-      <c r="C2" t="s">
-        <v>31</v>
-      </c>
       <c r="D2" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="14.5" x14ac:dyDescent="0.35">
@@ -891,7 +891,7 @@
         <v>14</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="14.5" x14ac:dyDescent="0.35">
@@ -899,42 +899,42 @@
         <v>7</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="14.5" x14ac:dyDescent="0.35">
       <c r="B5" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C5" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="C5" s="7" t="s">
-        <v>42</v>
-      </c>
       <c r="D5" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="14.5" x14ac:dyDescent="0.35">
       <c r="B6" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C6" s="7" t="s">
         <v>19</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="E7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="38.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="J9" s="12" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="K9" s="12"/>
     </row>
@@ -975,7 +975,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -1082,12 +1082,12 @@
     </row>
     <row r="7" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="G7" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="49.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H8" s="12" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I8" s="12"/>
     </row>

</xml_diff>

<commit_message>
Added test method to test with all options like Infant sitting options etc
</commit_message>
<xml_diff>
--- a/DataSheets/Data_sheets_expedia.xlsx
+++ b/DataSheets/Data_sheets_expedia.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Selenium\Selenium projects second\ExpediaMavenFramework\DataSheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6408D53E-FC28-42B5-A6D4-EC88CDA9272B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F67C147-1127-4587-A564-C591708DFF9A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Important Information" sheetId="6" r:id="rId1"/>
@@ -18,14 +18,15 @@
     <sheet name="OneWayFlightsPosDefaultDate" sheetId="4" r:id="rId3"/>
     <sheet name="OneWayFlightsPosDate" sheetId="5" r:id="rId4"/>
     <sheet name="OneWayFlightsWithTravellers" sheetId="1" r:id="rId5"/>
-    <sheet name="FlightsWithHotelsPositive" sheetId="2" r:id="rId6"/>
+    <sheet name="OneWayFlightsTravellersAge" sheetId="7" r:id="rId6"/>
+    <sheet name="FlightsWithHotelsPositive" sheetId="2" r:id="rId7"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="75">
   <si>
     <t>OneWayHotels</t>
   </si>
@@ -169,16 +170,7 @@
     <t>6 Jun 2021</t>
   </si>
   <si>
-    <t>3 May 2021</t>
-  </si>
-  <si>
-    <t>25 Apr 2021</t>
-  </si>
-  <si>
     <t>18 Aug 2021</t>
-  </si>
-  <si>
-    <t>28 Mar 2021</t>
   </si>
   <si>
     <t>OneWayTravellers</t>
@@ -224,9 +216,6 @@
     <t>12 Jun 2021</t>
   </si>
   <si>
-    <t>30 Mar 2021</t>
-  </si>
-  <si>
     <t>OneWayFlightsTravellersDate</t>
   </si>
   <si>
@@ -234,6 +223,76 @@
   </si>
   <si>
     <t>7 Jun 2021</t>
+  </si>
+  <si>
+    <t>ChildrenAges</t>
+  </si>
+  <si>
+    <t>InfantAges</t>
+  </si>
+  <si>
+    <t>OneWayTravellersAge</t>
+  </si>
+  <si>
+    <t>InfantSitting</t>
+  </si>
+  <si>
+    <t>Instruction - Put the start tag (OneWayTravellersAge) before the first column and the first row to be used and the end tag (OneWayTravellersAge) after the last column and last row to be used.
+Only use positive scenarios here.</t>
+  </si>
+  <si>
+    <t>As per the positive scenarios, please ensure the following:
+* Please limit the total number of travellers to 6.
+* If the infants sit on the lap, please provide equivalent number of children above 12 years or adults as the number of infants.
+* If you are providing only adults and infants, please ensure there are no more than 2 infants per adult.</t>
+  </si>
+  <si>
+    <t>ChildrenAge</t>
+  </si>
+  <si>
+    <t>12,8</t>
+  </si>
+  <si>
+    <t>Under 1,1</t>
+  </si>
+  <si>
+    <t>InfantAge(Under 1/1)</t>
+  </si>
+  <si>
+    <t>InfantSitting (seat/lap)</t>
+  </si>
+  <si>
+    <t>On lap,In seat</t>
+  </si>
+  <si>
+    <t>In seat</t>
+  </si>
+  <si>
+    <t>30 Aug 2021</t>
+  </si>
+  <si>
+    <t>25 May 2021</t>
+  </si>
+  <si>
+    <t>6,12</t>
+  </si>
+  <si>
+    <t>On Lap</t>
+  </si>
+  <si>
+    <t>Under 1, 1</t>
+  </si>
+  <si>
+    <t>in seat</t>
+  </si>
+  <si>
+    <t>28 Jul 2021</t>
+  </si>
+  <si>
+    <t>25 Aug 2021</t>
+  </si>
+  <si>
+    <t>31 May 2021</t>
   </si>
 </sst>
 </file>
@@ -547,7 +606,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03D385C2-6E58-432F-BCCC-55E697E10F02}">
   <dimension ref="A1:A8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:A8"/>
     </sheetView>
   </sheetViews>
@@ -558,7 +617,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="10" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
@@ -593,24 +652,24 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD5D1D3A-5071-4574-BCCD-29CCFD49D1EA}">
-  <dimension ref="A1:M11"/>
+  <dimension ref="A1:P11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="24.33203125" customWidth="1"/>
-    <col min="2" max="7" width="13.08203125" customWidth="1"/>
-    <col min="8" max="8" width="22.4140625" customWidth="1"/>
-    <col min="12" max="12" width="18" customWidth="1"/>
-    <col min="13" max="13" width="18.75" customWidth="1"/>
+    <col min="2" max="10" width="13.08203125" customWidth="1"/>
+    <col min="11" max="11" width="22.4140625" customWidth="1"/>
+    <col min="15" max="15" width="18" customWidth="1"/>
+    <col min="16" max="16" width="18.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:16" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A1" s="9" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -628,10 +687,19 @@
         <v>21</v>
       </c>
       <c r="G1" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="I1" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" ht="14.5" x14ac:dyDescent="0.35">
       <c r="B2" s="1" t="s">
         <v>13</v>
       </c>
@@ -639,7 +707,7 @@
         <v>4</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="E2">
         <v>2</v>
@@ -648,10 +716,19 @@
         <v>1</v>
       </c>
       <c r="G2">
+        <v>5</v>
+      </c>
+      <c r="H2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="I2">
+        <v>1</v>
+      </c>
+      <c r="J2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" ht="14.5" x14ac:dyDescent="0.35">
       <c r="B3" s="1" t="s">
         <v>12</v>
       </c>
@@ -659,19 +736,28 @@
         <v>16</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>44</v>
+        <v>67</v>
       </c>
       <c r="E3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F3">
+        <v>2</v>
+      </c>
+      <c r="G3" t="s">
+        <v>68</v>
+      </c>
+      <c r="H3">
         <v>1</v>
       </c>
-      <c r="G3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="I3">
+        <v>1</v>
+      </c>
+      <c r="J3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" ht="14.5" x14ac:dyDescent="0.35">
       <c r="B4" s="1" t="s">
         <v>18</v>
       </c>
@@ -679,19 +765,28 @@
         <v>7</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>53</v>
+        <v>66</v>
       </c>
       <c r="E4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F4">
         <v>1</v>
       </c>
       <c r="G4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
+        <v>10</v>
+      </c>
+      <c r="H4">
+        <v>2</v>
+      </c>
+      <c r="I4" t="s">
+        <v>70</v>
+      </c>
+      <c r="J4" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" ht="14.5" x14ac:dyDescent="0.35">
       <c r="B5" s="1" t="s">
         <v>7</v>
       </c>
@@ -699,7 +794,7 @@
         <v>14</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="E5">
         <v>1</v>
@@ -707,11 +802,11 @@
       <c r="F5">
         <v>0</v>
       </c>
-      <c r="G5">
+      <c r="H5">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:16" ht="14.5" x14ac:dyDescent="0.35">
       <c r="B6" s="1" t="s">
         <v>19</v>
       </c>
@@ -719,7 +814,7 @@
         <v>17</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="E6">
         <v>1</v>
@@ -727,29 +822,30 @@
       <c r="F6">
         <v>0</v>
       </c>
-      <c r="G6">
+      <c r="H6">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="H7" s="9" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" ht="54" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:16" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="K7" s="9" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" ht="54" customHeight="1" x14ac:dyDescent="0.3">
       <c r="F10" s="8"/>
-      <c r="L10" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="M10" s="12"/>
-    </row>
-    <row r="11" spans="1:13" ht="60.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="L11" s="12"/>
-      <c r="M11" s="12"/>
+      <c r="G10" s="8"/>
+      <c r="O10" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="P10" s="12"/>
+    </row>
+    <row r="11" spans="1:16" ht="60.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="O11" s="12"/>
+      <c r="P11" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="L10:M11"/>
+    <mergeCell ref="O10:P11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -824,7 +920,7 @@
     </row>
     <row r="9" spans="1:10" ht="33.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="I9" s="12" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="J9" s="12"/>
     </row>
@@ -845,7 +941,7 @@
   <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J9" sqref="J9:K10"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -880,7 +976,7 @@
         <v>29</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>46</v>
+        <v>72</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="14.5" x14ac:dyDescent="0.35">
@@ -891,7 +987,7 @@
         <v>14</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>44</v>
+        <v>73</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="14.5" x14ac:dyDescent="0.35">
@@ -913,7 +1009,7 @@
         <v>40</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>43</v>
+        <v>74</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="14.5" x14ac:dyDescent="0.35">
@@ -924,7 +1020,7 @@
         <v>19</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
@@ -934,7 +1030,7 @@
     </row>
     <row r="9" spans="1:11" ht="38.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="J9" s="12" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="K9" s="12"/>
     </row>
@@ -952,10 +1048,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I1000"/>
+  <dimension ref="A1:L1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H8" sqref="H8:I9"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -964,18 +1060,18 @@
     <col min="2" max="2" width="12.6640625" customWidth="1"/>
     <col min="3" max="3" width="15.6640625" customWidth="1"/>
     <col min="4" max="4" width="14.58203125" customWidth="1"/>
-    <col min="5" max="5" width="16.25" customWidth="1"/>
-    <col min="6" max="6" width="24.4140625" customWidth="1"/>
-    <col min="7" max="7" width="26.33203125" customWidth="1"/>
-    <col min="8" max="9" width="27.25" customWidth="1"/>
-    <col min="10" max="10" width="26.4140625" customWidth="1"/>
-    <col min="11" max="11" width="26" customWidth="1"/>
-    <col min="12" max="25" width="7.6640625" customWidth="1"/>
+    <col min="5" max="6" width="16.25" customWidth="1"/>
+    <col min="7" max="9" width="24.4140625" customWidth="1"/>
+    <col min="10" max="10" width="26.33203125" customWidth="1"/>
+    <col min="11" max="12" width="27.25" customWidth="1"/>
+    <col min="13" max="13" width="26.4140625" customWidth="1"/>
+    <col min="14" max="14" width="26" customWidth="1"/>
+    <col min="15" max="28" width="7.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -990,12 +1086,21 @@
         <v>21</v>
       </c>
       <c r="F1" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-    </row>
-    <row r="2" spans="1:9" ht="17" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H1" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+    </row>
+    <row r="2" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B2" s="1" t="s">
         <v>13</v>
       </c>
@@ -1008,11 +1113,14 @@
       <c r="E2">
         <v>1</v>
       </c>
-      <c r="F2">
+      <c r="G2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="I2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B3" s="1" t="s">
         <v>12</v>
       </c>
@@ -1026,10 +1134,13 @@
         <v>1</v>
       </c>
       <c r="F3">
+        <v>5</v>
+      </c>
+      <c r="G3">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B4" s="1" t="s">
         <v>18</v>
       </c>
@@ -1042,11 +1153,17 @@
       <c r="E4">
         <v>0</v>
       </c>
-      <c r="F4">
+      <c r="G4">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H4" t="s">
+        <v>61</v>
+      </c>
+      <c r="I4" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B5" s="1" t="s">
         <v>7</v>
       </c>
@@ -1059,11 +1176,14 @@
       <c r="E5">
         <v>2</v>
       </c>
-      <c r="F5">
+      <c r="F5" t="s">
+        <v>60</v>
+      </c>
+      <c r="G5">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B6" s="1" t="s">
         <v>19</v>
       </c>
@@ -1076,32 +1196,32 @@
       <c r="E6">
         <v>0</v>
       </c>
-      <c r="F6">
+      <c r="G6">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="G7" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="49.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="H8" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="I8" s="12"/>
-    </row>
-    <row r="9" spans="1:9" ht="27.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="H9" s="12"/>
-      <c r="I9" s="12"/>
-    </row>
-    <row r="10" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="11" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="12" spans="1:9" ht="31.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="13" spans="1:9" ht="46" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="14" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="15" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="16" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="7" spans="1:12" ht="14" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="J7" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="49.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="K8" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="L8" s="12"/>
+    </row>
+    <row r="9" spans="1:12" ht="27.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="K9" s="12"/>
+      <c r="L9" s="12"/>
+    </row>
+    <row r="10" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="11" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="12" spans="1:12" ht="31.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="13" spans="1:12" ht="46" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="14" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="15" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="16" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="17" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="18" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2088,7 +2208,7 @@
     <row r="1000" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="H8:I9"/>
+    <mergeCell ref="K8:L9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="portrait"/>
@@ -2096,6 +2216,175 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6D9BDD4-FD13-4686-873D-F52657C1C979}">
+  <dimension ref="A1:L11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="19.1640625" customWidth="1"/>
+    <col min="2" max="2" width="15.83203125" customWidth="1"/>
+    <col min="3" max="3" width="16.5" customWidth="1"/>
+    <col min="4" max="4" width="12.4140625" customWidth="1"/>
+    <col min="5" max="6" width="12.5" customWidth="1"/>
+    <col min="7" max="9" width="12.33203125" customWidth="1"/>
+    <col min="10" max="10" width="18.1640625" customWidth="1"/>
+    <col min="11" max="11" width="19.25" customWidth="1"/>
+    <col min="12" max="12" width="25" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+    </row>
+    <row r="2" spans="1:12" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="B2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2">
+        <v>2</v>
+      </c>
+      <c r="E2">
+        <v>2</v>
+      </c>
+      <c r="G2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="B3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3">
+        <v>4</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="B4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4">
+        <v>3</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="B5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5">
+        <v>3</v>
+      </c>
+      <c r="E5">
+        <v>2</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="B6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6">
+        <v>6</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="53.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="K8" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="L8" s="12"/>
+    </row>
+    <row r="9" spans="1:12" ht="58.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="K9" s="12"/>
+      <c r="L9" s="12"/>
+    </row>
+    <row r="10" spans="1:12" ht="62" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="K10" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="L10" s="11"/>
+    </row>
+    <row r="11" spans="1:12" ht="60.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="K11" s="11"/>
+      <c r="L11" s="11"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="K8:L9"/>
+    <mergeCell ref="K10:L11"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>

</xml_diff>

<commit_message>
Trucated the source and destination values to airport codes and removed inbuilt dates for the functional sheets.
</commit_message>
<xml_diff>
--- a/DataSheets/Data_sheets_expedia.xlsx
+++ b/DataSheets/Data_sheets_expedia.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Selenium\Selenium projects second\ExpediaMavenFramework\DataSheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F67C147-1127-4587-A564-C591708DFF9A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6608C8CB-89F5-4841-86F8-B9934E753622}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Important Information" sheetId="6" r:id="rId1"/>
-    <sheet name="OneWayFlightsPosTrvDate" sheetId="3" r:id="rId2"/>
+    <sheet name="OneWayFlightsPosAllOptions" sheetId="3" r:id="rId2"/>
     <sheet name="OneWayFlightsPosDefaultDate" sheetId="4" r:id="rId3"/>
     <sheet name="OneWayFlightsPosDate" sheetId="5" r:id="rId4"/>
     <sheet name="OneWayFlightsWithTravellers" sheetId="1" r:id="rId5"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="72">
   <si>
     <t>OneWayHotels</t>
   </si>
@@ -35,9 +35,6 @@
   </si>
   <si>
     <t>Destination</t>
-  </si>
-  <si>
-    <t>(Date in dd/mm/yyyy format)</t>
   </si>
   <si>
     <t>Mumbai</t>
@@ -125,52 +122,10 @@
     <t>06/09/2020</t>
   </si>
   <si>
-    <t>Kozhikode</t>
-  </si>
-  <si>
-    <t>Dubai</t>
-  </si>
-  <si>
     <t>OneWayFlightsPos</t>
   </si>
   <si>
     <t>OneWayFlightsPosDate</t>
-  </si>
-  <si>
-    <t>Date</t>
-  </si>
-  <si>
-    <t>Hyderabad</t>
-  </si>
-  <si>
-    <t>New Delhi</t>
-  </si>
-  <si>
-    <t>Bangkok</t>
-  </si>
-  <si>
-    <t>Kolkata</t>
-  </si>
-  <si>
-    <t>Tokyo</t>
-  </si>
-  <si>
-    <t>Chicago</t>
-  </si>
-  <si>
-    <t>Bangalore</t>
-  </si>
-  <si>
-    <t>Bombay</t>
-  </si>
-  <si>
-    <t>Bhubaneswar</t>
-  </si>
-  <si>
-    <t>6 Jun 2021</t>
-  </si>
-  <si>
-    <t>18 Aug 2021</t>
   </si>
   <si>
     <t>OneWayTravellers</t>
@@ -213,16 +168,7 @@
     </r>
   </si>
   <si>
-    <t>12 Jun 2021</t>
-  </si>
-  <si>
     <t>OneWayFlightsTravellersDate</t>
-  </si>
-  <si>
-    <t>19 Nov 2021</t>
-  </si>
-  <si>
-    <t>7 Jun 2021</t>
   </si>
   <si>
     <t>ChildrenAges</t>
@@ -262,18 +208,9 @@
     <t>InfantSitting (seat/lap)</t>
   </si>
   <si>
-    <t>On lap,In seat</t>
-  </si>
-  <si>
     <t>In seat</t>
   </si>
   <si>
-    <t>30 Aug 2021</t>
-  </si>
-  <si>
-    <t>25 May 2021</t>
-  </si>
-  <si>
     <t>6,12</t>
   </si>
   <si>
@@ -286,13 +223,67 @@
     <t>in seat</t>
   </si>
   <si>
-    <t>28 Jul 2021</t>
-  </si>
-  <si>
-    <t>25 Aug 2021</t>
-  </si>
-  <si>
-    <t>31 May 2021</t>
+    <t>FlightClass</t>
+  </si>
+  <si>
+    <t>Economy</t>
+  </si>
+  <si>
+    <t>Premium Economy</t>
+  </si>
+  <si>
+    <t>Business Class</t>
+  </si>
+  <si>
+    <t>First Class</t>
+  </si>
+  <si>
+    <t>CCJ</t>
+  </si>
+  <si>
+    <t>DXB</t>
+  </si>
+  <si>
+    <t>BOM</t>
+  </si>
+  <si>
+    <t>TRV</t>
+  </si>
+  <si>
+    <t>MAA</t>
+  </si>
+  <si>
+    <t>ORD</t>
+  </si>
+  <si>
+    <t>BLR</t>
+  </si>
+  <si>
+    <t>DEL</t>
+  </si>
+  <si>
+    <t>BBI</t>
+  </si>
+  <si>
+    <t>HYD</t>
+  </si>
+  <si>
+    <t>LON</t>
+  </si>
+  <si>
+    <t>BKK</t>
+  </si>
+  <si>
+    <t>CCU</t>
+  </si>
+  <si>
+    <t>TYO</t>
+  </si>
+  <si>
+    <t>Under 1</t>
+  </si>
+  <si>
+    <t>On lap</t>
   </si>
 </sst>
 </file>
@@ -366,14 +357,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -606,7 +596,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03D385C2-6E58-432F-BCCC-55E697E10F02}">
   <dimension ref="A1:A8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:A8"/>
     </sheetView>
   </sheetViews>
@@ -616,30 +606,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1" s="10" t="s">
-        <v>48</v>
+      <c r="A1" s="9" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" s="11"/>
+      <c r="A2" s="10"/>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A3" s="11"/>
+      <c r="A3" s="10"/>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A4" s="11"/>
+      <c r="A4" s="10"/>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A5" s="11"/>
+      <c r="A5" s="10"/>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A6" s="11"/>
+      <c r="A6" s="10"/>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A7" s="11"/>
+      <c r="A7" s="10"/>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A8" s="11"/>
+      <c r="A8" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -654,22 +644,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD5D1D3A-5071-4574-BCCD-29CCFD49D1EA}">
   <dimension ref="A1:P11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="24.33203125" customWidth="1"/>
-    <col min="2" max="10" width="13.08203125" customWidth="1"/>
+    <col min="2" max="9" width="13.08203125" customWidth="1"/>
+    <col min="10" max="10" width="17.9140625" customWidth="1"/>
     <col min="11" max="11" width="22.4140625" customWidth="1"/>
     <col min="15" max="15" width="18" customWidth="1"/>
     <col min="16" max="16" width="18.75" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="9" t="s">
-        <v>50</v>
+      <c r="A1" s="8" t="s">
+        <v>34</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -677,171 +668,168 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
+      <c r="D1" s="2" t="s">
+        <v>19</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>20</v>
       </c>
       <c r="F1" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="G1" s="2" t="s">
-        <v>53</v>
-      </c>
       <c r="H1" s="2" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>54</v>
+        <v>38</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:16" ht="14.5" x14ac:dyDescent="0.35">
       <c r="B2" s="1" t="s">
-        <v>13</v>
+        <v>62</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>49</v>
+        <v>58</v>
+      </c>
+      <c r="D2">
+        <v>2</v>
       </c>
       <c r="E2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F2">
+        <v>5</v>
+      </c>
+      <c r="G2">
         <v>1</v>
-      </c>
-      <c r="G2">
-        <v>5</v>
       </c>
       <c r="H2">
         <v>1</v>
       </c>
-      <c r="I2">
-        <v>1</v>
+      <c r="I2" t="s">
+        <v>46</v>
       </c>
       <c r="J2" t="s">
-        <v>65</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:16" ht="14.5" x14ac:dyDescent="0.35">
       <c r="B3" s="1" t="s">
-        <v>12</v>
+        <v>64</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>67</v>
+        <v>65</v>
+      </c>
+      <c r="D3">
+        <v>3</v>
       </c>
       <c r="E3">
-        <v>3</v>
-      </c>
-      <c r="F3">
         <v>2</v>
       </c>
-      <c r="G3" t="s">
-        <v>68</v>
+      <c r="F3" t="s">
+        <v>47</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
       </c>
       <c r="H3">
         <v>1</v>
       </c>
-      <c r="I3">
-        <v>1</v>
+      <c r="I3" t="s">
+        <v>48</v>
       </c>
       <c r="J3" t="s">
-        <v>69</v>
+        <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:16" ht="14.5" x14ac:dyDescent="0.35">
       <c r="B4" s="1" t="s">
-        <v>18</v>
+        <v>63</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>66</v>
+        <v>60</v>
+      </c>
+      <c r="D4">
+        <v>2</v>
       </c>
       <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>10</v>
+      </c>
+      <c r="G4">
         <v>2</v>
       </c>
-      <c r="F4">
-        <v>1</v>
-      </c>
-      <c r="G4">
-        <v>10</v>
-      </c>
-      <c r="H4">
-        <v>2</v>
+      <c r="H4" t="s">
+        <v>49</v>
       </c>
       <c r="I4" t="s">
-        <v>70</v>
+        <v>50</v>
       </c>
       <c r="J4" t="s">
-        <v>71</v>
+        <v>54</v>
       </c>
     </row>
     <row r="5" spans="1:16" ht="14.5" x14ac:dyDescent="0.35">
       <c r="B5" s="1" t="s">
-        <v>7</v>
+        <v>60</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>51</v>
+        <v>59</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
       </c>
       <c r="E5">
-        <v>1</v>
-      </c>
-      <c r="F5">
         <v>0</v>
       </c>
-      <c r="H5">
+      <c r="G5">
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:16" ht="14.5" x14ac:dyDescent="0.35">
       <c r="B6" s="1" t="s">
-        <v>19</v>
+        <v>63</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>52</v>
+        <v>58</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
       </c>
       <c r="E6">
-        <v>1</v>
-      </c>
-      <c r="F6">
         <v>0</v>
       </c>
-      <c r="H6">
+      <c r="G6">
         <v>0</v>
       </c>
+      <c r="J6" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="7" spans="1:16" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="K7" s="9" t="s">
-        <v>50</v>
+      <c r="K7" s="8" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:16" ht="54" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F10" s="8"/>
-      <c r="G10" s="8"/>
-      <c r="O10" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="P10" s="12"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+      <c r="O10" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="P10" s="11"/>
     </row>
     <row r="11" spans="1:16" ht="60.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="O11" s="12"/>
-      <c r="P11" s="12"/>
+      <c r="O11" s="11"/>
+      <c r="P11" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -857,7 +845,7 @@
   <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I9" sqref="I9:J10"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -872,7 +860,7 @@
   <sheetData>
     <row r="1" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -883,50 +871,50 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
-        <v>28</v>
+        <v>56</v>
       </c>
       <c r="C2" t="s">
-        <v>29</v>
+        <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B3" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>10</v>
+      <c r="B3" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B4" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>35</v>
+      <c r="B4" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B5" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>37</v>
+      <c r="B5" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="D6" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="33.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="I9" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="J9" s="12"/>
+      <c r="I9" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="J9" s="11"/>
     </row>
     <row r="10" spans="1:10" ht="73" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="I10" s="12"/>
-      <c r="J10" s="12"/>
+      <c r="I10" s="11"/>
+      <c r="J10" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -938,25 +926,25 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A0505F9-B8CF-4B2F-A121-89B24FCC7D64}">
-  <dimension ref="A1:K10"/>
+  <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="22.9140625" customWidth="1"/>
     <col min="2" max="2" width="12" customWidth="1"/>
-    <col min="3" max="4" width="14.33203125" customWidth="1"/>
-    <col min="5" max="5" width="23.5" customWidth="1"/>
-    <col min="10" max="10" width="18.4140625" customWidth="1"/>
-    <col min="11" max="11" width="13.6640625" customWidth="1"/>
+    <col min="3" max="3" width="21.83203125" customWidth="1"/>
+    <col min="4" max="4" width="23.5" customWidth="1"/>
+    <col min="9" max="9" width="18.4140625" customWidth="1"/>
+    <col min="10" max="10" width="13.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -964,83 +952,65 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" ht="14.5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B3" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B4" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B5" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B6" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="D7" t="s">
         <v>28</v>
       </c>
-      <c r="C2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="B3" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="B4" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="B5" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="B6" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="E7" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" ht="38.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="J9" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="K9" s="12"/>
-    </row>
-    <row r="10" spans="1:11" ht="58.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="J10" s="12"/>
-      <c r="K10" s="12"/>
+    </row>
+    <row r="9" spans="1:10" ht="38.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I9" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="J9" s="11"/>
+    </row>
+    <row r="10" spans="1:10" ht="58.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I10" s="11"/>
+      <c r="J10" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="J9:K10"/>
+    <mergeCell ref="I9:J10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1050,8 +1020,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView topLeftCell="F1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1071,7 +1041,7 @@
   <sheetData>
     <row r="1" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -1080,32 +1050,32 @@
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="F1" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="H1" s="2" t="s">
-        <v>62</v>
+        <v>44</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>63</v>
+        <v>45</v>
       </c>
       <c r="J1" s="2"/>
       <c r="K1" s="2"/>
     </row>
     <row r="2" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B2" s="1" t="s">
-        <v>13</v>
+        <v>62</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>4</v>
+        <v>58</v>
       </c>
       <c r="D2">
         <v>2</v>
@@ -1113,19 +1083,25 @@
       <c r="E2">
         <v>1</v>
       </c>
+      <c r="F2">
+        <v>7</v>
+      </c>
       <c r="G2">
         <v>1</v>
       </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
       <c r="I2" t="s">
-        <v>65</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B3" s="1" t="s">
-        <v>12</v>
+        <v>64</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>16</v>
+        <v>65</v>
       </c>
       <c r="D3">
         <v>4</v>
@@ -1139,13 +1115,16 @@
       <c r="G3">
         <v>1</v>
       </c>
+      <c r="H3" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="4" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B4" s="1" t="s">
-        <v>18</v>
+        <v>63</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>7</v>
+        <v>60</v>
       </c>
       <c r="D4">
         <v>3</v>
@@ -1157,18 +1136,18 @@
         <v>2</v>
       </c>
       <c r="H4" t="s">
-        <v>61</v>
+        <v>43</v>
       </c>
       <c r="I4" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B5" s="1" t="s">
-        <v>7</v>
+        <v>60</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>14</v>
+        <v>59</v>
       </c>
       <c r="D5">
         <v>3</v>
@@ -1177,18 +1156,21 @@
         <v>2</v>
       </c>
       <c r="F5" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="G5">
         <v>1</v>
       </c>
+      <c r="H5" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="6" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B6" s="1" t="s">
-        <v>19</v>
+        <v>63</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>17</v>
+        <v>58</v>
       </c>
       <c r="D6">
         <v>6</v>
@@ -1202,18 +1184,18 @@
     </row>
     <row r="7" spans="1:12" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="J7" s="1" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="49.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="K8" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="L8" s="12"/>
+      <c r="K8" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="L8" s="11"/>
     </row>
     <row r="9" spans="1:12" ht="27.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="K9" s="12"/>
-      <c r="L9" s="12"/>
+      <c r="K9" s="11"/>
+      <c r="L9" s="11"/>
     </row>
     <row r="10" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="11" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2238,7 +2220,7 @@
   <sheetData>
     <row r="1" spans="1:12" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>55</v>
+        <v>37</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -2247,32 +2229,32 @@
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="F1" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="H1" s="2" t="s">
-        <v>54</v>
+        <v>36</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>56</v>
+        <v>38</v>
       </c>
       <c r="J1" s="2"/>
       <c r="K1" s="2"/>
     </row>
     <row r="2" spans="1:12" ht="14.5" x14ac:dyDescent="0.35">
       <c r="B2" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D2">
         <v>2</v>
@@ -2286,10 +2268,10 @@
     </row>
     <row r="3" spans="1:12" ht="14.5" x14ac:dyDescent="0.35">
       <c r="B3" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D3">
         <v>4</v>
@@ -2301,15 +2283,15 @@
         <v>1</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>55</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="14.5" x14ac:dyDescent="0.35">
       <c r="B4" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D4">
         <v>3</v>
@@ -2323,10 +2305,10 @@
     </row>
     <row r="5" spans="1:12" ht="14.5" x14ac:dyDescent="0.35">
       <c r="B5" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D5">
         <v>3</v>
@@ -2340,10 +2322,10 @@
     </row>
     <row r="6" spans="1:12" ht="14.5" x14ac:dyDescent="0.35">
       <c r="B6" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D6">
         <v>6</v>
@@ -2356,24 +2338,24 @@
       </c>
     </row>
     <row r="8" spans="1:12" ht="53.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="K8" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="L8" s="12"/>
+      <c r="K8" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="L8" s="11"/>
     </row>
     <row r="9" spans="1:12" ht="58.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="K9" s="12"/>
-      <c r="L9" s="12"/>
+      <c r="K9" s="11"/>
+      <c r="L9" s="11"/>
     </row>
     <row r="10" spans="1:12" ht="62" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="K10" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="L10" s="11"/>
+      <c r="K10" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="L10" s="10"/>
     </row>
     <row r="11" spans="1:12" ht="60.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="K11" s="11"/>
-      <c r="L11" s="11"/>
+      <c r="K11" s="10"/>
+      <c r="L11" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -2416,47 +2398,47 @@
         <v>2</v>
       </c>
       <c r="D1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>6</v>
-      </c>
       <c r="F1" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="B2" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E2" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="F2" s="5" t="s">
         <v>26</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="B3" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D3" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="E3" s="5" t="s">
-        <v>26</v>
-      </c>
       <c r="F3" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>0</v>
@@ -2464,31 +2446,31 @@
     </row>
     <row r="4" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="B4" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="14" x14ac:dyDescent="0.3"/>
     <row r="11" spans="1:8" ht="49.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G11" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="H11" s="12"/>
+      <c r="G11" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="H11" s="11"/>
     </row>
     <row r="12" spans="1:8" ht="34" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G12" s="12"/>
-      <c r="H12" s="12"/>
+      <c r="G12" s="11"/>
+      <c r="H12" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Added code for return flights testing.
</commit_message>
<xml_diff>
--- a/DataSheets/Data_sheets_expedia.xlsx
+++ b/DataSheets/Data_sheets_expedia.xlsx
@@ -1,32 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Selenium\Selenium projects second\ExpediaMavenFramework\DataSheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6608C8CB-89F5-4841-86F8-B9934E753622}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EAC1DD3-8064-4886-A21D-91B09B263439}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Important Information" sheetId="6" r:id="rId1"/>
     <sheet name="OneWayFlightsPosAllOptions" sheetId="3" r:id="rId2"/>
-    <sheet name="OneWayFlightsPosDefaultDate" sheetId="4" r:id="rId3"/>
+    <sheet name="FlightsPosDefaultDate" sheetId="4" r:id="rId3"/>
     <sheet name="OneWayFlightsPosDate" sheetId="5" r:id="rId4"/>
     <sheet name="OneWayFlightsWithTravellers" sheetId="1" r:id="rId5"/>
-    <sheet name="OneWayFlightsTravellersAge" sheetId="7" r:id="rId6"/>
-    <sheet name="FlightsWithHotelsPositive" sheetId="2" r:id="rId7"/>
+    <sheet name="FlightsWithHotelsPositive" sheetId="2" r:id="rId6"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="63">
   <si>
     <t>OneWayHotels</t>
   </si>
@@ -46,9 +45,6 @@
     <t>Hotel Check-in Date (in dd/mm/yyyy)</t>
   </si>
   <si>
-    <t>Chennai</t>
-  </si>
-  <si>
     <t>Hotel Check-out Date (in dd/mm/yyyy)</t>
   </si>
   <si>
@@ -61,22 +57,7 @@
     <t>07/12/2019</t>
   </si>
   <si>
-    <t>Bhubaneshwar</t>
-  </si>
-  <si>
-    <t>Bengaluru</t>
-  </si>
-  <si>
-    <t>Trivandrum</t>
-  </si>
-  <si>
     <t>new york</t>
-  </si>
-  <si>
-    <t>hyderabad</t>
-  </si>
-  <si>
-    <t>mumbai</t>
   </si>
   <si>
     <t>delhi</t>
@@ -122,9 +103,6 @@
     <t>06/09/2020</t>
   </si>
   <si>
-    <t>OneWayFlightsPos</t>
-  </si>
-  <si>
     <t>OneWayFlightsPosDate</t>
   </si>
   <si>
@@ -143,147 +121,116 @@
 Only use positive scenarios here.</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">All sheets with the word 'Pos' within their tab name indicate test data for positive test cases. If one of the columns in any of those sheets contains date, ensure to provide only current or future dates. </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Don't provide past dates else the test will fail.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">
+    <t>OneWayFlightsTravellersDate</t>
+  </si>
+  <si>
+    <t>ChildrenAges</t>
+  </si>
+  <si>
+    <t>InfantAges</t>
+  </si>
+  <si>
+    <t>InfantSitting</t>
+  </si>
+  <si>
+    <t>ChildrenAge</t>
+  </si>
+  <si>
+    <t>12,8</t>
+  </si>
+  <si>
+    <t>Under 1,1</t>
+  </si>
+  <si>
+    <t>InfantAge(Under 1/1)</t>
+  </si>
+  <si>
+    <t>InfantSitting (seat/lap)</t>
+  </si>
+  <si>
+    <t>In seat</t>
+  </si>
+  <si>
+    <t>6,12</t>
+  </si>
+  <si>
+    <t>On Lap</t>
+  </si>
+  <si>
+    <t>Under 1, 1</t>
+  </si>
+  <si>
+    <t>in seat</t>
+  </si>
+  <si>
+    <t>FlightClass</t>
+  </si>
+  <si>
+    <t>Economy</t>
+  </si>
+  <si>
+    <t>Premium Economy</t>
+  </si>
+  <si>
+    <t>Business Class</t>
+  </si>
+  <si>
+    <t>First Class</t>
+  </si>
+  <si>
+    <t>CCJ</t>
+  </si>
+  <si>
+    <t>DXB</t>
+  </si>
+  <si>
+    <t>BOM</t>
+  </si>
+  <si>
+    <t>TRV</t>
+  </si>
+  <si>
+    <t>MAA</t>
+  </si>
+  <si>
+    <t>ORD</t>
+  </si>
+  <si>
+    <t>BLR</t>
+  </si>
+  <si>
+    <t>DEL</t>
+  </si>
+  <si>
+    <t>BBI</t>
+  </si>
+  <si>
+    <t>HYD</t>
+  </si>
+  <si>
+    <t>LON</t>
+  </si>
+  <si>
+    <t>BKK</t>
+  </si>
+  <si>
+    <t>CCU</t>
+  </si>
+  <si>
+    <t>TYO</t>
+  </si>
+  <si>
+    <t>Under 1</t>
+  </si>
+  <si>
+    <t>On lap</t>
+  </si>
+  <si>
+    <t>All sheets with the word 'Pos' within their tab name indicate test data for positive test cases.
 Look out for specific instruction in each sheet.</t>
-    </r>
-  </si>
-  <si>
-    <t>OneWayFlightsTravellersDate</t>
-  </si>
-  <si>
-    <t>ChildrenAges</t>
-  </si>
-  <si>
-    <t>InfantAges</t>
-  </si>
-  <si>
-    <t>OneWayTravellersAge</t>
-  </si>
-  <si>
-    <t>InfantSitting</t>
-  </si>
-  <si>
-    <t>Instruction - Put the start tag (OneWayTravellersAge) before the first column and the first row to be used and the end tag (OneWayTravellersAge) after the last column and last row to be used.
-Only use positive scenarios here.</t>
-  </si>
-  <si>
-    <t>As per the positive scenarios, please ensure the following:
-* Please limit the total number of travellers to 6.
-* If the infants sit on the lap, please provide equivalent number of children above 12 years or adults as the number of infants.
-* If you are providing only adults and infants, please ensure there are no more than 2 infants per adult.</t>
-  </si>
-  <si>
-    <t>ChildrenAge</t>
-  </si>
-  <si>
-    <t>12,8</t>
-  </si>
-  <si>
-    <t>Under 1,1</t>
-  </si>
-  <si>
-    <t>InfantAge(Under 1/1)</t>
-  </si>
-  <si>
-    <t>InfantSitting (seat/lap)</t>
-  </si>
-  <si>
-    <t>In seat</t>
-  </si>
-  <si>
-    <t>6,12</t>
-  </si>
-  <si>
-    <t>On Lap</t>
-  </si>
-  <si>
-    <t>Under 1, 1</t>
-  </si>
-  <si>
-    <t>in seat</t>
-  </si>
-  <si>
-    <t>FlightClass</t>
-  </si>
-  <si>
-    <t>Economy</t>
-  </si>
-  <si>
-    <t>Premium Economy</t>
-  </si>
-  <si>
-    <t>Business Class</t>
-  </si>
-  <si>
-    <t>First Class</t>
-  </si>
-  <si>
-    <t>CCJ</t>
-  </si>
-  <si>
-    <t>DXB</t>
-  </si>
-  <si>
-    <t>BOM</t>
-  </si>
-  <si>
-    <t>TRV</t>
-  </si>
-  <si>
-    <t>MAA</t>
-  </si>
-  <si>
-    <t>ORD</t>
-  </si>
-  <si>
-    <t>BLR</t>
-  </si>
-  <si>
-    <t>DEL</t>
-  </si>
-  <si>
-    <t>BBI</t>
-  </si>
-  <si>
-    <t>HYD</t>
-  </si>
-  <si>
-    <t>LON</t>
-  </si>
-  <si>
-    <t>BKK</t>
-  </si>
-  <si>
-    <t>CCU</t>
-  </si>
-  <si>
-    <t>TYO</t>
-  </si>
-  <si>
-    <t>Under 1</t>
-  </si>
-  <si>
-    <t>On lap</t>
+  </si>
+  <si>
+    <t>FlightsDefaultDtPos</t>
   </si>
 </sst>
 </file>
@@ -607,7 +554,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
-        <v>33</v>
+        <v>61</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
@@ -644,7 +591,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD5D1D3A-5071-4574-BCCD-29CCFD49D1EA}">
   <dimension ref="A1:P11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
       <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
@@ -660,7 +607,7 @@
   <sheetData>
     <row r="1" spans="1:16" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A1" s="8" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -669,33 +616,33 @@
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:16" ht="14.5" x14ac:dyDescent="0.35">
       <c r="B2" s="1" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="D2">
         <v>2</v>
@@ -713,18 +660,18 @@
         <v>1</v>
       </c>
       <c r="I2" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="J2" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:16" ht="14.5" x14ac:dyDescent="0.35">
       <c r="B3" s="1" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
       <c r="D3">
         <v>3</v>
@@ -733,7 +680,7 @@
         <v>2</v>
       </c>
       <c r="F3" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="G3">
         <v>1</v>
@@ -742,18 +689,18 @@
         <v>1</v>
       </c>
       <c r="I3" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="J3" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:16" ht="14.5" x14ac:dyDescent="0.35">
       <c r="B4" s="1" t="s">
-        <v>63</v>
+        <v>52</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
       <c r="D4">
         <v>2</v>
@@ -768,21 +715,21 @@
         <v>2</v>
       </c>
       <c r="H4" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="I4" t="s">
-        <v>50</v>
+        <v>39</v>
       </c>
       <c r="J4" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:16" ht="14.5" x14ac:dyDescent="0.35">
       <c r="B5" s="1" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -796,10 +743,10 @@
     </row>
     <row r="6" spans="1:16" ht="14.5" x14ac:dyDescent="0.35">
       <c r="B6" s="1" t="s">
-        <v>63</v>
+        <v>52</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -811,19 +758,19 @@
         <v>0</v>
       </c>
       <c r="J6" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:16" ht="14.5" x14ac:dyDescent="0.35">
       <c r="K7" s="8" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:16" ht="54" customHeight="1" x14ac:dyDescent="0.3">
       <c r="E10" s="7"/>
       <c r="F10" s="7"/>
       <c r="O10" s="11" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="P10" s="11"/>
     </row>
@@ -845,7 +792,7 @@
   <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="I9" sqref="I9:J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -860,7 +807,7 @@
   <sheetData>
     <row r="1" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>27</v>
+        <v>62</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -871,44 +818,44 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="C2" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B3" s="6" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B4" s="6" t="s">
-        <v>63</v>
+        <v>52</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B5" s="6" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="D6" t="s">
-        <v>27</v>
+        <v>62</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="33.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="I9" s="11" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="J9" s="11"/>
     </row>
@@ -944,7 +891,7 @@
   <sheetData>
     <row r="1" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -955,52 +902,52 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="C2" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B3" s="6" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B4" s="6" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B5" s="6" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B6" s="6" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>63</v>
+        <v>52</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="D7" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="38.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="I9" s="11" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="J9" s="11"/>
     </row>
@@ -1020,7 +967,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L1000"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
@@ -1041,7 +988,7 @@
   <sheetData>
     <row r="1" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -1050,32 +997,32 @@
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="J1" s="2"/>
       <c r="K1" s="2"/>
     </row>
     <row r="2" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B2" s="1" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="D2">
         <v>2</v>
@@ -1093,15 +1040,15 @@
         <v>1</v>
       </c>
       <c r="I2" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B3" s="1" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
       <c r="D3">
         <v>4</v>
@@ -1116,15 +1063,15 @@
         <v>1</v>
       </c>
       <c r="H3" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B4" s="1" t="s">
-        <v>63</v>
+        <v>52</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
       <c r="D4">
         <v>3</v>
@@ -1136,18 +1083,18 @@
         <v>2</v>
       </c>
       <c r="H4" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="I4" t="s">
-        <v>71</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B5" s="1" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="D5">
         <v>3</v>
@@ -1156,21 +1103,21 @@
         <v>2</v>
       </c>
       <c r="F5" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
       <c r="G5">
         <v>1</v>
       </c>
       <c r="H5" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B6" s="1" t="s">
-        <v>63</v>
+        <v>52</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="D6">
         <v>6</v>
@@ -1184,12 +1131,12 @@
     </row>
     <row r="7" spans="1:12" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="J7" s="1" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="49.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="K8" s="11" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="L8" s="11"/>
     </row>
@@ -2198,175 +2145,6 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6D9BDD4-FD13-4686-873D-F52657C1C979}">
-  <dimension ref="A1:L11"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="19.1640625" customWidth="1"/>
-    <col min="2" max="2" width="15.83203125" customWidth="1"/>
-    <col min="3" max="3" width="16.5" customWidth="1"/>
-    <col min="4" max="4" width="12.4140625" customWidth="1"/>
-    <col min="5" max="6" width="12.5" customWidth="1"/>
-    <col min="7" max="9" width="12.33203125" customWidth="1"/>
-    <col min="10" max="10" width="18.1640625" customWidth="1"/>
-    <col min="11" max="11" width="19.25" customWidth="1"/>
-    <col min="12" max="12" width="25" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:12" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-    </row>
-    <row r="2" spans="1:12" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="B2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2">
-        <v>2</v>
-      </c>
-      <c r="E2">
-        <v>2</v>
-      </c>
-      <c r="G2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="B3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3">
-        <v>4</v>
-      </c>
-      <c r="E3">
-        <v>1</v>
-      </c>
-      <c r="G3">
-        <v>1</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="B4" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4">
-        <v>3</v>
-      </c>
-      <c r="E4">
-        <v>0</v>
-      </c>
-      <c r="G4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="B5" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5">
-        <v>3</v>
-      </c>
-      <c r="E5">
-        <v>2</v>
-      </c>
-      <c r="G5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="B6" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D6">
-        <v>6</v>
-      </c>
-      <c r="E6">
-        <v>0</v>
-      </c>
-      <c r="G6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" ht="53.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="K8" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="L8" s="11"/>
-    </row>
-    <row r="9" spans="1:12" ht="58.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="K9" s="11"/>
-      <c r="L9" s="11"/>
-    </row>
-    <row r="10" spans="1:12" ht="62" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="K10" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="L10" s="10"/>
-    </row>
-    <row r="11" spans="1:12" ht="60.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="K11" s="10"/>
-      <c r="L11" s="10"/>
-    </row>
-  </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="K8:L9"/>
-    <mergeCell ref="K10:L11"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -2404,24 +2182,24 @@
         <v>5</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="B2" s="2" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
@@ -2429,16 +2207,16 @@
         <v>3</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>0</v>
@@ -2446,25 +2224,25 @@
     </row>
     <row r="4" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="B4" s="2" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="14" x14ac:dyDescent="0.3"/>
     <row r="11" spans="1:8" ht="49.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G11" s="12" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="H11" s="11"/>
     </row>

</xml_diff>

<commit_message>
Added a return flight test case with depart and return dates.
</commit_message>
<xml_diff>
--- a/DataSheets/Data_sheets_expedia.xlsx
+++ b/DataSheets/Data_sheets_expedia.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Selenium\Selenium projects second\ExpediaMavenFramework\DataSheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EAC1DD3-8064-4886-A21D-91B09B263439}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE983C04-3612-481A-8510-B1915E4C8369}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Important Information" sheetId="6" r:id="rId1"/>
     <sheet name="OneWayFlightsPosAllOptions" sheetId="3" r:id="rId2"/>
     <sheet name="FlightsPosDefaultDate" sheetId="4" r:id="rId3"/>
-    <sheet name="OneWayFlightsPosDate" sheetId="5" r:id="rId4"/>
+    <sheet name="FlightsPosDate" sheetId="5" r:id="rId4"/>
     <sheet name="OneWayFlightsWithTravellers" sheetId="1" r:id="rId5"/>
     <sheet name="FlightsWithHotelsPositive" sheetId="2" r:id="rId6"/>
   </sheets>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="64">
   <si>
     <t>OneWayHotels</t>
   </si>
@@ -103,14 +103,7 @@
     <t>06/09/2020</t>
   </si>
   <si>
-    <t>OneWayFlightsPosDate</t>
-  </si>
-  <si>
     <t>OneWayTravellers</t>
-  </si>
-  <si>
-    <t>Instruction - Put the start tag (OneWayFlightsPosDate) before the first column and the first row to be used and the end tag (OneWayFlightsPosDate) after the last column and last row to be used.
-Only use positive scenarios here.</t>
   </si>
   <si>
     <t>Instruction - Put the start tag (OneWayTravellers) before the first column and the first row to be used and the end tag (OneWayTravellers) after the last column and last row to be used.
@@ -231,6 +224,17 @@
   </si>
   <si>
     <t>FlightsDefaultDtPos</t>
+  </si>
+  <si>
+    <t>Instruction - Put the start tag (FlightsDefaultDtPos) before the first column and the first row to be used and the end tag (FlightsDefaultDtPos) after the last column and last row to be used.
+Only use positive scenarios here.</t>
+  </si>
+  <si>
+    <t>FlightsPosWithDate</t>
+  </si>
+  <si>
+    <t>Instruction - Put the start tag (FlightsPosWithDate) before the first column and the first row to be used and the end tag (FlightsPosWithDate) after the last column and last row to be used.
+Only use positive scenarios here.</t>
   </si>
 </sst>
 </file>
@@ -554,7 +558,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
@@ -591,7 +595,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD5D1D3A-5071-4574-BCCD-29CCFD49D1EA}">
   <dimension ref="A1:P11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+    <sheetView topLeftCell="D1" workbookViewId="0">
       <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
@@ -607,7 +611,7 @@
   <sheetData>
     <row r="1" spans="1:16" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A1" s="8" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -622,27 +626,27 @@
         <v>14</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>15</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:16" ht="14.5" x14ac:dyDescent="0.35">
       <c r="B2" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D2">
         <v>2</v>
@@ -660,18 +664,18 @@
         <v>1</v>
       </c>
       <c r="I2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="J2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:16" ht="14.5" x14ac:dyDescent="0.35">
       <c r="B3" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D3">
         <v>3</v>
@@ -680,7 +684,7 @@
         <v>2</v>
       </c>
       <c r="F3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G3">
         <v>1</v>
@@ -689,18 +693,18 @@
         <v>1</v>
       </c>
       <c r="I3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="J3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:16" ht="14.5" x14ac:dyDescent="0.35">
       <c r="B4" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D4">
         <v>2</v>
@@ -715,21 +719,21 @@
         <v>2</v>
       </c>
       <c r="H4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="I4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="J4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:16" ht="14.5" x14ac:dyDescent="0.35">
       <c r="B5" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -743,10 +747,10 @@
     </row>
     <row r="6" spans="1:16" ht="14.5" x14ac:dyDescent="0.35">
       <c r="B6" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -758,19 +762,19 @@
         <v>0</v>
       </c>
       <c r="J6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="7" spans="1:16" ht="14.5" x14ac:dyDescent="0.35">
       <c r="K7" s="8" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:16" ht="54" customHeight="1" x14ac:dyDescent="0.3">
       <c r="E10" s="7"/>
       <c r="F10" s="7"/>
       <c r="O10" s="11" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="P10" s="11"/>
     </row>
@@ -807,7 +811,7 @@
   <sheetData>
     <row r="1" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -818,44 +822,44 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B3" s="6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B4" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B5" s="6" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="D6" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="33.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="I9" s="11" t="s">
-        <v>25</v>
+        <v>61</v>
       </c>
       <c r="J9" s="11"/>
     </row>
@@ -875,8 +879,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A0505F9-B8CF-4B2F-A121-89B24FCC7D64}">
   <dimension ref="A1:J10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -891,7 +895,7 @@
   <sheetData>
     <row r="1" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>21</v>
+        <v>62</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -902,52 +906,52 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B3" s="6" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B4" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B5" s="6" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B6" s="6" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="D7" t="s">
-        <v>21</v>
+        <v>62</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="38.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="I9" s="11" t="s">
-        <v>23</v>
+        <v>63</v>
       </c>
       <c r="J9" s="11"/>
     </row>
@@ -988,7 +992,7 @@
   <sheetData>
     <row r="1" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -1003,26 +1007,26 @@
         <v>14</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>15</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J1" s="2"/>
       <c r="K1" s="2"/>
     </row>
     <row r="2" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B2" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D2">
         <v>2</v>
@@ -1040,15 +1044,15 @@
         <v>1</v>
       </c>
       <c r="I2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B3" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D3">
         <v>4</v>
@@ -1063,15 +1067,15 @@
         <v>1</v>
       </c>
       <c r="H3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B4" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D4">
         <v>3</v>
@@ -1083,18 +1087,18 @@
         <v>2</v>
       </c>
       <c r="H4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="I4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B5" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D5">
         <v>3</v>
@@ -1103,21 +1107,21 @@
         <v>2</v>
       </c>
       <c r="F5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="G5">
         <v>1</v>
       </c>
       <c r="H5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B6" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D6">
         <v>6</v>
@@ -1131,12 +1135,12 @@
     </row>
     <row r="7" spans="1:12" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="J7" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="49.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="K8" s="11" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="L8" s="11"/>
     </row>

</xml_diff>

<commit_message>
Implemented a WebDriverFactory class for customized webdrivers.
</commit_message>
<xml_diff>
--- a/DataSheets/Data_sheets_expedia.xlsx
+++ b/DataSheets/Data_sheets_expedia.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Selenium\Selenium projects second\ExpediaMavenFramework\DataSheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE983C04-3612-481A-8510-B1915E4C8369}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E45F3E5D-BE0D-4675-952A-3BB7F9D54C4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -880,7 +880,7 @@
   <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>

</xml_diff>